<commit_message>
Update Data and Export to Excel (writexl)
</commit_message>
<xml_diff>
--- a/data/Sensory Profile.xlsx
+++ b/data/Sensory Profile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thier\Documents\R\Intro 2 Data Science\thierry_code\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thier\Documents\R\i2ds4scc_bookdown\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E87BEB-5D66-4063-B402-C6D04EA7C0F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12075B1C-7C78-4985-8AC0-713A31232419}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-4350" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="5310" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -229,9 +229,6 @@
     <t>Astringent</t>
   </si>
   <si>
-    <t>Raw dough flavor</t>
-  </si>
-  <si>
     <t>Dairy flavor</t>
   </si>
   <si>
@@ -380,6 +377,9 @@
   </si>
   <si>
     <t>J09</t>
+  </si>
+  <si>
+    <t>RawDough flavor</t>
   </si>
 </sst>
 </file>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92187ACC-497E-45B8-BD96-2A9FCB4E84F8}">
   <dimension ref="A1:AI100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="154.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -842,105 +842,105 @@
         <v>35</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>62</v>
-      </c>
       <c r="L1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="N1" s="15" t="s">
-        <v>51</v>
-      </c>
       <c r="O1" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P1" s="15" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="Q1" s="15" t="s">
         <v>37</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S1" s="15" t="s">
         <v>38</v>
       </c>
       <c r="T1" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U1" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="W1" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="X1" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="X1" s="15" t="s">
-        <v>66</v>
       </c>
       <c r="Y1" s="15" t="s">
         <v>44</v>
       </c>
       <c r="Z1" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AA1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF1" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AG1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE1" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF1" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AI1" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="AI1" s="15" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>20</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="3" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>21</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>22</v>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>23</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>24</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>25</v>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>26</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>28</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>29</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>30</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -2117,7 +2117,7 @@
     </row>
     <row r="13" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>20</v>
@@ -2224,7 +2224,7 @@
     </row>
     <row r="14" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>21</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="15" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>22</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="16" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>23</v>
@@ -2545,7 +2545,7 @@
     </row>
     <row r="17" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>24</v>
@@ -2652,7 +2652,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>25</v>
@@ -2759,7 +2759,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>28</v>
@@ -2973,7 +2973,7 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>29</v>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="22" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>30</v>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
@@ -3294,7 +3294,7 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>20</v>
@@ -3401,7 +3401,7 @@
     </row>
     <row r="25" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>21</v>
@@ -3508,7 +3508,7 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>22</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>23</v>
@@ -3722,7 +3722,7 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>24</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>25</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>26</v>
@@ -4043,7 +4043,7 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>28</v>
@@ -4150,7 +4150,7 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>29</v>
@@ -4257,7 +4257,7 @@
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>30</v>
@@ -4364,7 +4364,7 @@
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
         <v>18</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>20</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>21</v>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>22</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>23</v>
@@ -4899,7 +4899,7 @@
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>24</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>25</v>
@@ -5113,7 +5113,7 @@
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>26</v>
@@ -5220,7 +5220,7 @@
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>28</v>
@@ -5327,7 +5327,7 @@
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>29</v>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>30</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
         <v>18</v>
@@ -5648,7 +5648,7 @@
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>20</v>
@@ -5755,7 +5755,7 @@
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>21</v>
@@ -5862,7 +5862,7 @@
     </row>
     <row r="48" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A48" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>22</v>
@@ -5969,7 +5969,7 @@
     </row>
     <row r="49" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A49" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>23</v>
@@ -6076,7 +6076,7 @@
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>24</v>
@@ -6183,7 +6183,7 @@
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>25</v>
@@ -6290,7 +6290,7 @@
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>26</v>
@@ -6397,7 +6397,7 @@
     </row>
     <row r="53" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A53" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>28</v>
@@ -6504,7 +6504,7 @@
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>29</v>
@@ -6611,7 +6611,7 @@
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>30</v>
@@ -6718,7 +6718,7 @@
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56" t="s">
         <v>18</v>
@@ -6825,7 +6825,7 @@
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>20</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>21</v>
@@ -7039,7 +7039,7 @@
     </row>
     <row r="59" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A59" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>22</v>
@@ -7146,7 +7146,7 @@
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>23</v>
@@ -7253,7 +7253,7 @@
     </row>
     <row r="61" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A61" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>24</v>
@@ -7360,7 +7360,7 @@
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>25</v>
@@ -7467,7 +7467,7 @@
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>26</v>
@@ -7574,7 +7574,7 @@
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>28</v>
@@ -7681,7 +7681,7 @@
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>29</v>
@@ -7788,7 +7788,7 @@
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>30</v>
@@ -7895,7 +7895,7 @@
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
         <v>18</v>
@@ -8002,7 +8002,7 @@
     </row>
     <row r="68" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A68" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>20</v>
@@ -8109,7 +8109,7 @@
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>21</v>
@@ -8216,7 +8216,7 @@
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>22</v>
@@ -8323,7 +8323,7 @@
     </row>
     <row r="71" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>23</v>
@@ -8430,7 +8430,7 @@
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>24</v>
@@ -8537,7 +8537,7 @@
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>25</v>
@@ -8644,7 +8644,7 @@
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>26</v>
@@ -8751,7 +8751,7 @@
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>28</v>
@@ -8858,7 +8858,7 @@
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>29</v>
@@ -8965,7 +8965,7 @@
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>30</v>
@@ -9072,7 +9072,7 @@
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
         <v>18</v>
@@ -9179,7 +9179,7 @@
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>20</v>
@@ -9286,7 +9286,7 @@
     </row>
     <row r="80" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A80" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>21</v>
@@ -9393,7 +9393,7 @@
     </row>
     <row r="81" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>22</v>
@@ -9500,7 +9500,7 @@
     </row>
     <row r="82" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A82" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>23</v>
@@ -9607,7 +9607,7 @@
     </row>
     <row r="83" spans="1:35" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A83" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>24</v>
@@ -9714,7 +9714,7 @@
     </row>
     <row r="84" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>25</v>
@@ -9821,7 +9821,7 @@
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>26</v>
@@ -9928,7 +9928,7 @@
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>28</v>
@@ -10035,7 +10035,7 @@
     </row>
     <row r="87" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>29</v>
@@ -10142,7 +10142,7 @@
     </row>
     <row r="88" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>30</v>
@@ -10249,7 +10249,7 @@
     </row>
     <row r="89" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B89" t="s">
         <v>18</v>
@@ -10356,7 +10356,7 @@
     </row>
     <row r="90" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>20</v>
@@ -10463,7 +10463,7 @@
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>21</v>
@@ -10570,7 +10570,7 @@
     </row>
     <row r="92" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>22</v>
@@ -10677,7 +10677,7 @@
     </row>
     <row r="93" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>23</v>
@@ -10784,7 +10784,7 @@
     </row>
     <row r="94" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>24</v>
@@ -10891,7 +10891,7 @@
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>25</v>
@@ -10998,7 +10998,7 @@
     </row>
     <row r="96" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>26</v>
@@ -11105,7 +11105,7 @@
     </row>
     <row r="97" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>28</v>
@@ -11212,7 +11212,7 @@
     </row>
     <row r="98" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>29</v>
@@ -11319,7 +11319,7 @@
     </row>
     <row r="99" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>30</v>
@@ -11426,7 +11426,7 @@
     </row>
     <row r="100" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B100" t="s">
         <v>18</v>
@@ -11556,22 +11556,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="D1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -11585,13 +11585,13 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -11605,13 +11605,13 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -11625,13 +11625,13 @@
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -11645,13 +11645,13 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -11665,13 +11665,13 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -11685,13 +11685,13 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -11705,13 +11705,13 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -11725,13 +11725,13 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -11745,13 +11745,13 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -11765,13 +11765,13 @@
         <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -11785,13 +11785,13 @@
         <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -11806,7 +11806,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.86328125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -11819,13 +11819,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -11845,7 +11845,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>32</v>
@@ -11856,7 +11856,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>32</v>
@@ -11867,7 +11867,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>32</v>
@@ -11878,7 +11878,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>32</v>
@@ -11889,7 +11889,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>32</v>
@@ -11900,7 +11900,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>32</v>
@@ -11911,7 +11911,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>32</v>
@@ -11922,7 +11922,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>32</v>
@@ -11933,7 +11933,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>36</v>
@@ -11944,7 +11944,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>36</v>
@@ -11955,7 +11955,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>36</v>
@@ -11966,7 +11966,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>39</v>
@@ -11977,7 +11977,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>39</v>
@@ -11999,7 +11999,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>39</v>
@@ -12021,7 +12021,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>39</v>
@@ -12032,7 +12032,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>39</v>
@@ -12043,7 +12043,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>39</v>
@@ -12054,7 +12054,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>39</v>
@@ -12065,7 +12065,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>39</v>
@@ -12087,7 +12087,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>39</v>
@@ -12098,7 +12098,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>33</v>
@@ -12109,7 +12109,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>33</v>
@@ -12120,7 +12120,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>33</v>
@@ -12131,7 +12131,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>33</v>
@@ -12142,7 +12142,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>33</v>
@@ -12153,7 +12153,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>33</v>
@@ -12164,7 +12164,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>33</v>
@@ -12175,7 +12175,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>33</v>
@@ -12186,7 +12186,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
Include text for full_join()
</commit_message>
<xml_diff>
--- a/data/Sensory Profile.xlsx
+++ b/data/Sensory Profile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thier\Documents\R\i2ds4scc_bookdown\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12075B1C-7C78-4985-8AC0-713A31232419}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D519713-9C76-453C-8C95-89D98A7E1188}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="5310" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="5310" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="97">
   <si>
     <t>P01</t>
   </si>
@@ -380,6 +380,9 @@
   </si>
   <si>
     <t>RawDough flavor</t>
+  </si>
+  <si>
+    <t>Popt</t>
   </si>
 </sst>
 </file>
@@ -789,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92187ACC-497E-45B8-BD96-2A9FCB4E84F8}">
   <dimension ref="A1:AI100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="154.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -11539,10 +11542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -11554,7 +11557,7 @@
     <col min="6" max="6" width="17.06640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="13.15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
@@ -11574,7 +11577,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -11594,7 +11597,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -11614,7 +11617,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -11634,7 +11637,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -11654,7 +11657,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -11674,7 +11677,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -11694,7 +11697,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -11714,7 +11717,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -11734,7 +11737,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -11754,7 +11757,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -11774,7 +11777,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -11792,6 +11795,9 @@
       </c>
       <c r="F12" t="s">
         <v>77</v>
+      </c>
+      <c r="G12" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update dataset and auto-report section on openxlsx
</commit_message>
<xml_diff>
--- a/data/Sensory Profile.xlsx
+++ b/data/Sensory Profile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thier\Documents\R\i2ds4scc_bookdown\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B1F0A51-5E4D-459F-B70B-DE7AE05ED244}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3141EE48-673F-4B73-A513-CB1C17C1A1F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="5310" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Color evenness</t>
-  </si>
-  <si>
-    <t>Qtt of inclusions</t>
   </si>
   <si>
     <t>Surface defects</t>
@@ -115,9 +112,6 @@
   </si>
   <si>
     <t>Dry in mouth</t>
-  </si>
-  <si>
-    <t>Qtt of inclusions in mouth</t>
   </si>
   <si>
     <t>Sticky</t>
@@ -241,6 +235,12 @@
   </si>
   <si>
     <t>In-mouth</t>
+  </si>
+  <si>
+    <t>Qty of inclusions in mouth</t>
+  </si>
+  <si>
+    <t>Qty of inclusions</t>
   </si>
 </sst>
 </file>
@@ -680,10 +680,46 @@
   <dimension ref="A1:AH100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.53125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.265625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.53125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
@@ -702,99 +738,99 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2">
         <v>48.6</v>
@@ -895,10 +931,10 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
       </c>
       <c r="C3" s="2">
         <v>46.2</v>
@@ -999,10 +1035,10 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="2">
         <v>48</v>
@@ -1103,10 +1139,10 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2">
         <v>5.4</v>
@@ -1207,10 +1243,10 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1311,10 +1347,10 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -1415,10 +1451,10 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
         <v>4.8</v>
@@ -1519,10 +1555,10 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -1623,10 +1659,10 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -1727,10 +1763,10 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2">
         <v>52.8</v>
@@ -1831,10 +1867,10 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2">
         <v>53.4</v>
@@ -1935,10 +1971,10 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2">
         <v>39.6</v>
@@ -2039,10 +2075,10 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2">
         <v>36</v>
@@ -2143,10 +2179,10 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2">
         <v>36</v>
@@ -2247,10 +2283,10 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2">
         <v>41.4</v>
@@ -2351,10 +2387,10 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
@@ -2455,10 +2491,10 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2">
         <v>5.4</v>
@@ -2559,10 +2595,10 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>10.199999999999999</v>
@@ -2663,10 +2699,10 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2">
         <v>0</v>
@@ -2767,10 +2803,10 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2">
         <v>13.8</v>
@@ -2871,10 +2907,10 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="2">
         <v>44.4</v>
@@ -2975,10 +3011,10 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2">
         <v>13.8</v>
@@ -3079,10 +3115,10 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C24" s="2">
         <v>39</v>
@@ -3183,10 +3219,10 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C25" s="2">
         <v>48</v>
@@ -3287,10 +3323,10 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C26" s="2">
         <v>35.4</v>
@@ -3391,10 +3427,10 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C27" s="2">
         <v>37.200000000000003</v>
@@ -3495,10 +3531,10 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C28" s="2">
         <v>0</v>
@@ -3599,10 +3635,10 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="2">
         <v>35.4</v>
@@ -3703,10 +3739,10 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" s="2">
         <v>36</v>
@@ -3807,10 +3843,10 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C31" s="2">
         <v>21</v>
@@ -3911,10 +3947,10 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -4015,10 +4051,10 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="2">
         <v>40.200000000000003</v>
@@ -4119,10 +4155,10 @@
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C34" s="2">
         <v>34.200000000000003</v>
@@ -4223,10 +4259,10 @@
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" s="2">
         <v>39.6</v>
@@ -4327,10 +4363,10 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C36" s="2">
         <v>38.4</v>
@@ -4431,10 +4467,10 @@
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" s="2">
         <v>15</v>
@@ -4535,10 +4571,10 @@
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" s="2">
         <v>30.6</v>
@@ -4639,10 +4675,10 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" s="2">
         <v>0</v>
@@ -4743,10 +4779,10 @@
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" s="2">
         <v>10.199999999999999</v>
@@ -4847,10 +4883,10 @@
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C41" s="2">
         <v>12</v>
@@ -4951,10 +4987,10 @@
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2">
         <v>7.8</v>
@@ -5055,10 +5091,10 @@
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43" s="2">
         <v>0</v>
@@ -5159,10 +5195,10 @@
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44" s="2">
         <v>37.799999999999997</v>
@@ -5263,10 +5299,10 @@
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C45" s="2">
         <v>16.2</v>
@@ -5367,10 +5403,10 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C46" s="2">
         <v>33.6</v>
@@ -5471,10 +5507,10 @@
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C47" s="2">
         <v>47.4</v>
@@ -5575,10 +5611,10 @@
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C48" s="2">
         <v>37.200000000000003</v>
@@ -5679,10 +5715,10 @@
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C49" s="2">
         <v>46.2</v>
@@ -5783,10 +5819,10 @@
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C50" s="2">
         <v>9.6</v>
@@ -5887,10 +5923,10 @@
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C51" s="2">
         <v>21</v>
@@ -5991,10 +6027,10 @@
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C52" s="2">
         <v>17.399999999999999</v>
@@ -6095,10 +6131,10 @@
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C53" s="2">
         <v>13.8</v>
@@ -6199,10 +6235,10 @@
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C54" s="2">
         <v>7.8</v>
@@ -6303,10 +6339,10 @@
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C55" s="2">
         <v>43.8</v>
@@ -6407,10 +6443,10 @@
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C56" s="2">
         <v>36</v>
@@ -6511,10 +6547,10 @@
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C57" s="2">
         <v>38.4</v>
@@ -6615,10 +6651,10 @@
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C58" s="2">
         <v>37.799999999999997</v>
@@ -6719,10 +6755,10 @@
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C59" s="2">
         <v>33</v>
@@ -6823,10 +6859,10 @@
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B60" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C60" s="2">
         <v>26.4</v>
@@ -6927,10 +6963,10 @@
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C61" s="2">
         <v>9</v>
@@ -7031,10 +7067,10 @@
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C62" s="2">
         <v>17.399999999999999</v>
@@ -7135,10 +7171,10 @@
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C63" s="2">
         <v>13.2</v>
@@ -7239,10 +7275,10 @@
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C64" s="2">
         <v>15</v>
@@ -7343,10 +7379,10 @@
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C65" s="2">
         <v>21</v>
@@ -7447,10 +7483,10 @@
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C66" s="2">
         <v>43.2</v>
@@ -7551,10 +7587,10 @@
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C67" s="2">
         <v>32.4</v>
@@ -7655,10 +7691,10 @@
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B68" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C68" s="2">
         <v>25.8</v>
@@ -7759,10 +7795,10 @@
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B69" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C69" s="2">
         <v>27</v>
@@ -7863,10 +7899,10 @@
     </row>
     <row r="70" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C70" s="2">
         <v>16.2</v>
@@ -7967,10 +8003,10 @@
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B71" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C71" s="2">
         <v>28.2</v>
@@ -8071,10 +8107,10 @@
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B72" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C72" s="2">
         <v>6.6</v>
@@ -8175,10 +8211,10 @@
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B73" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C73" s="2">
         <v>0</v>
@@ -8279,10 +8315,10 @@
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C74" s="2">
         <v>10.199999999999999</v>
@@ -8383,10 +8419,10 @@
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B75" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C75" s="2">
         <v>0</v>
@@ -8487,10 +8523,10 @@
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C76" s="2">
         <v>5.4</v>
@@ -8591,10 +8627,10 @@
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B77" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C77" s="2">
         <v>44.4</v>
@@ -8695,10 +8731,10 @@
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B78" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C78" s="2">
         <v>3</v>
@@ -8799,10 +8835,10 @@
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B79" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C79" s="2">
         <v>47.4</v>
@@ -8903,10 +8939,10 @@
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C80" s="2">
         <v>54</v>
@@ -9007,10 +9043,10 @@
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B81" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C81" s="2">
         <v>15</v>
@@ -9111,10 +9147,10 @@
     </row>
     <row r="82" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B82" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C82" s="2">
         <v>29.4</v>
@@ -9215,10 +9251,10 @@
     </row>
     <row r="83" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B83" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C83" s="2">
         <v>0</v>
@@ -9319,10 +9355,10 @@
     </row>
     <row r="84" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B84" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C84" s="2">
         <v>15</v>
@@ -9423,10 +9459,10 @@
     </row>
     <row r="85" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C85" s="2">
         <v>17.399999999999999</v>
@@ -9527,10 +9563,10 @@
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B86" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C86" s="2">
         <v>10.8</v>
@@ -9631,10 +9667,10 @@
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C87" s="2">
         <v>7.2</v>
@@ -9735,10 +9771,10 @@
     </row>
     <row r="88" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B88" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C88" s="2">
         <v>25.2</v>
@@ -9839,10 +9875,10 @@
     </row>
     <row r="89" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B89" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C89" s="2">
         <v>20.399999999999999</v>
@@ -9943,10 +9979,10 @@
     </row>
     <row r="90" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B90" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C90" s="2">
         <v>40.200000000000003</v>
@@ -10047,10 +10083,10 @@
     </row>
     <row r="91" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B91" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C91" s="2">
         <v>48.6</v>
@@ -10151,10 +10187,10 @@
     </row>
     <row r="92" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B92" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C92" s="2">
         <v>39</v>
@@ -10255,10 +10291,10 @@
     </row>
     <row r="93" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B93" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C93" s="2">
         <v>47.4</v>
@@ -10359,10 +10395,10 @@
     </row>
     <row r="94" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B94" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C94" s="2">
         <v>6.6</v>
@@ -10463,10 +10499,10 @@
     </row>
     <row r="95" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B95" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C95" s="2">
         <v>21</v>
@@ -10567,10 +10603,10 @@
     </row>
     <row r="96" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B96" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C96" s="2">
         <v>30.6</v>
@@ -10671,10 +10707,10 @@
     </row>
     <row r="97" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C97" s="2">
         <v>12</v>
@@ -10775,10 +10811,10 @@
     </row>
     <row r="98" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B98" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C98" s="2">
         <v>6.6</v>
@@ -10879,10 +10915,10 @@
     </row>
     <row r="99" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B99" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C99" s="2">
         <v>45.6</v>
@@ -10983,10 +11019,10 @@
     </row>
     <row r="100" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B100" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C100" s="2">
         <v>25.8</v>
@@ -11105,167 +11141,167 @@
         <v>1</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
         <v>58</v>
       </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -11279,25 +11315,25 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
@@ -11319,10 +11355,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -11330,10 +11366,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -11341,329 +11377,329 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="12" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>